<commit_message>
Llama Scout and maverick fot generated TDD
</commit_message>
<xml_diff>
--- a/results/test phase/result.xlsx
+++ b/results/test phase/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/GitHub/BLP25-Task-2/results/test phase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB04308F-81B4-A540-888C-9B8E8EFAB640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2A8D4B-62FA-0540-9080-771B63EE608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="800" windowWidth="28480" windowHeight="17300" xr2:uid="{8277C5D4-4CA4-9343-A068-9845D89C3C55}"/>
+    <workbookView xWindow="1200" yWindow="800" windowWidth="28480" windowHeight="17300" activeTab="1" xr2:uid="{8277C5D4-4CA4-9343-A068-9845D89C3C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Compilation</t>
+  </si>
+  <si>
+    <t>TDD Generated Tests</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627ACA8F-3F11-ED4E-AE6A-FF98F35EC729}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,10 +472,10 @@
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="5" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +488,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -499,8 +505,11 @@
       <c r="D2" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -513,8 +522,11 @@
       <c r="D3" s="1">
         <v>12.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -527,8 +539,11 @@
       <c r="D4" s="1">
         <v>34.200000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -541,8 +556,11 @@
       <c r="D5" s="1">
         <v>45.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -555,8 +573,11 @@
       <c r="D6" s="1">
         <v>54.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -569,8 +590,11 @@
       <c r="D7" s="1">
         <v>41.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -583,8 +607,11 @@
       <c r="D8" s="1">
         <v>46.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -605,10 +632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCAA2B6-7EF0-8741-ADB2-84B2199C13C4}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +644,7 @@
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,8 +663,13 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -665,8 +697,17 @@
       <c r="J2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -697,8 +738,17 @@
       <c r="J3">
         <v>192</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>214</v>
+      </c>
+      <c r="L3">
+        <v>46</v>
+      </c>
+      <c r="M3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -729,8 +779,17 @@
       <c r="J4">
         <v>305</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>230</v>
+      </c>
+      <c r="L4">
+        <v>41</v>
+      </c>
+      <c r="M4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -761,8 +820,17 @@
       <c r="J5">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>234</v>
+      </c>
+      <c r="L5">
+        <v>41</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -793,8 +861,17 @@
       <c r="J6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>196</v>
+      </c>
+      <c r="L6">
+        <v>28</v>
+      </c>
+      <c r="M6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -825,8 +902,17 @@
       <c r="J7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>191</v>
+      </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -857,8 +943,17 @@
       <c r="J8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>170</v>
+      </c>
+      <c r="L8">
+        <v>67</v>
+      </c>
+      <c r="M8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -889,8 +984,17 @@
       <c r="J9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>188</v>
+      </c>
+      <c r="L9">
+        <v>49</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -923,10 +1027,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TDD Given test added for scout and maverick
</commit_message>
<xml_diff>
--- a/results/test phase/result.xlsx
+++ b/results/test phase/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/GitHub/BLP25-Task-2/results/test phase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2A8D4B-62FA-0540-9080-771B63EE608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920BB3C4-2458-BD4C-A967-8BAF7E632190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="800" windowWidth="28480" windowHeight="17300" activeTab="1" xr2:uid="{8277C5D4-4CA4-9343-A068-9845D89C3C55}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>TDD Generated Tests</t>
+  </si>
+  <si>
+    <t>TDD Given Test</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627ACA8F-3F11-ED4E-AE6A-FF98F35EC729}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,7 +478,7 @@
     <col min="5" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +494,11 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -509,7 +515,7 @@
         <v>39.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -526,7 +532,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -543,7 +549,7 @@
         <v>44.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -559,8 +565,11 @@
       <c r="E5" s="1">
         <v>51.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1">
+        <v>67.599999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -576,8 +585,11 @@
       <c r="E6" s="1">
         <v>54.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>74.400000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -594,7 +606,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -611,7 +623,7 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -632,19 +644,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCAA2B6-7EF0-8741-ADB2-84B2199C13C4}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,8 +681,13 @@
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -706,8 +724,17 @@
       <c r="M2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -748,7 +775,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -789,7 +816,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -830,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -870,8 +897,17 @@
       <c r="M6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <v>149</v>
+      </c>
+      <c r="O6">
+        <v>9</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -911,8 +947,17 @@
       <c r="M7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <v>119</v>
+      </c>
+      <c r="O7">
+        <v>9</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -953,7 +998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -994,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1027,11 +1072,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>